<commit_message>
ProduccionDigital: Actualización de formatos
MA0501, MA0701, MA0801
</commit_message>
<xml_diff>
--- a/seguimiento/ProduccionDigital/SegDigital_MA_05_01_CO.xlsx
+++ b/seguimiento/ProduccionDigital/SegDigital_MA_05_01_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\Matematicas\seguimiento\ProduccionDigital\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Documents\Aula Planeta Colombia\Repositorios\Matematicas\seguimiento\ProduccionDigital\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="67">
   <si>
     <t>Cuaderno de estudio</t>
   </si>
@@ -116,9 +116,6 @@
     <t>Guión:</t>
   </si>
   <si>
-    <t>Carga de esqueleto a GRECO</t>
-  </si>
-  <si>
     <t>MA_05_01_CO</t>
   </si>
   <si>
@@ -206,12 +203,6 @@
     <t>REC250</t>
   </si>
   <si>
-    <t>Validación y desbloqueo</t>
-  </si>
-  <si>
-    <t>Notificación de disponibilidad</t>
-  </si>
-  <si>
     <t>Descarga de componente</t>
   </si>
   <si>
@@ -230,7 +221,10 @@
     <t>Desbloqueo y notificación</t>
   </si>
   <si>
-    <t>24/03/2015 06:08p.m.</t>
+    <t>Carga y validación de esqueleto</t>
+  </si>
+  <si>
+    <t>Asistente Digital</t>
   </si>
 </sst>
 </file>
@@ -240,7 +234,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,8 +287,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -319,8 +329,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -343,11 +359,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -385,14 +438,26 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -674,32 +739,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G4" sqref="G4:G29"/>
+      <selection pane="topRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="7.796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.73046875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="59.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.53125" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.3984375" style="1" customWidth="1"/>
-    <col min="5" max="8" width="12.06640625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.6640625" style="1"/>
+    <col min="5" max="7" width="12.06640625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18.100000000000001" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" ht="18.100000000000001" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>29</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" s="2" customFormat="1" ht="21.15" x14ac:dyDescent="0.45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="19"/>
+    </row>
+    <row r="3" spans="1:14" s="2" customFormat="1" ht="21.15" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>23</v>
       </c>
@@ -713,66 +787,60 @@
         <v>26</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="F3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="J3" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="J3" s="6" t="s">
+      <c r="K3" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="L3" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="K3" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>66</v>
-      </c>
+      <c r="M3" s="3"/>
       <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-    </row>
-    <row r="4" spans="1:15" ht="15.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="15" t="s">
+    </row>
+    <row r="4" spans="1:14" ht="15.85" x14ac:dyDescent="0.45">
+      <c r="A4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="7"/>
       <c r="D4" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="15">
         <v>42087.62777777778</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="15">
         <v>42087.663194444445</v>
       </c>
-      <c r="G4" s="14" t="s">
-        <v>68</v>
-      </c>
+      <c r="G4" s="9"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="14"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="K4" s="14"/>
+      <c r="L4" s="15"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>28</v>
@@ -780,22 +848,21 @@
       <c r="D5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="9"/>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="14"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="K5" s="14"/>
+      <c r="L5" s="15"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>28</v>
@@ -803,22 +870,21 @@
       <c r="D6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="14"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="K6" s="14"/>
+      <c r="L6" s="15"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>28</v>
@@ -826,22 +892,21 @@
       <c r="D7" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="9"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="14"/>
-    </row>
-    <row r="8" spans="1:15" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="K7" s="14"/>
+      <c r="L7" s="15"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>28</v>
@@ -849,22 +914,21 @@
       <c r="D8" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="14"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="K8" s="14"/>
+      <c r="L8" s="15"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>28</v>
@@ -872,22 +936,21 @@
       <c r="D9" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="14"/>
-    </row>
-    <row r="10" spans="1:15" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="K9" s="14"/>
+      <c r="L9" s="15"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>28</v>
@@ -895,22 +958,21 @@
       <c r="D10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="9"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="14"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="K10" s="14"/>
+      <c r="L10" s="15"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>28</v>
@@ -918,22 +980,21 @@
       <c r="D11" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="14"/>
-    </row>
-    <row r="12" spans="1:15" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="K11" s="14"/>
+      <c r="L11" s="15"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>28</v>
@@ -941,22 +1002,21 @@
       <c r="D12" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="14"/>
-    </row>
-    <row r="13" spans="1:15" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="K12" s="14"/>
+      <c r="L12" s="15"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A13" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>28</v>
@@ -964,22 +1024,21 @@
       <c r="D13" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="14"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="K13" s="14"/>
+      <c r="L13" s="15"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A14" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>28</v>
@@ -987,22 +1046,21 @@
       <c r="D14" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="14"/>
-    </row>
-    <row r="15" spans="1:15" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="K14" s="14"/>
+      <c r="L14" s="15"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A15" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>28</v>
@@ -1010,22 +1068,21 @@
       <c r="D15" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="9"/>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="14"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="K15" s="14"/>
+      <c r="L15" s="15"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A16" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>28</v>
@@ -1033,22 +1090,21 @@
       <c r="D16" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="9"/>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="14"/>
-    </row>
-    <row r="17" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="K16" s="14"/>
+      <c r="L16" s="15"/>
+    </row>
+    <row r="17" spans="1:12" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A17" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>28</v>
@@ -1056,22 +1112,21 @@
       <c r="D17" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="9"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="14"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="K17" s="14"/>
+      <c r="L17" s="15"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A18" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>28</v>
@@ -1079,22 +1134,21 @@
       <c r="D18" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="9"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="14"/>
-    </row>
-    <row r="19" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="K18" s="14"/>
+      <c r="L18" s="15"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A19" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>28</v>
@@ -1102,22 +1156,21 @@
       <c r="D19" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="9"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="14"/>
-    </row>
-    <row r="20" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="K19" s="14"/>
+      <c r="L19" s="15"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A20" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>28</v>
@@ -1125,22 +1178,21 @@
       <c r="D20" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="9"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="14"/>
-    </row>
-    <row r="21" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="K20" s="14"/>
+      <c r="L20" s="15"/>
+    </row>
+    <row r="21" spans="1:12" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A21" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>28</v>
@@ -1148,22 +1200,21 @@
       <c r="D21" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="9"/>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="14"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="K21" s="14"/>
+      <c r="L21" s="15"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A22" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>28</v>
@@ -1171,22 +1222,21 @@
       <c r="D22" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="9"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="14"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="K22" s="14"/>
+      <c r="L22" s="15"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A23" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>28</v>
@@ -1194,22 +1244,21 @@
       <c r="D23" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="9"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="14"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="K23" s="14"/>
+      <c r="L23" s="15"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A24" s="10" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>28</v>
@@ -1217,22 +1266,21 @@
       <c r="D24" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="9"/>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="14"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="K24" s="14"/>
+      <c r="L24" s="15"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A25" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>28</v>
@@ -1240,22 +1288,21 @@
       <c r="D25" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="9"/>
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="14"/>
-    </row>
-    <row r="26" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="K25" s="14"/>
+      <c r="L25" s="15"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A26" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>28</v>
@@ -1263,22 +1310,21 @@
       <c r="D26" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="9"/>
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
       <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="14"/>
-    </row>
-    <row r="27" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="K26" s="14"/>
+      <c r="L26" s="15"/>
+    </row>
+    <row r="27" spans="1:12" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A27" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>28</v>
@@ -1286,19 +1332,18 @@
       <c r="D27" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="9"/>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
       <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="14"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="K27" s="14"/>
+      <c r="L27" s="15"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A28" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>1</v>
@@ -1309,22 +1354,21 @@
       <c r="D28" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="9"/>
       <c r="H28" s="9"/>
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="14"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="K28" s="14"/>
+      <c r="L28" s="15"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A29" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>28</v>
@@ -1332,24 +1376,23 @@
       <c r="D29" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="9"/>
       <c r="H29" s="9"/>
       <c r="I29" s="9"/>
       <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="G2:K2"/>
     <mergeCell ref="A4:B4"/>
+    <mergeCell ref="K4:K29"/>
     <mergeCell ref="L4:L29"/>
-    <mergeCell ref="M4:M29"/>
     <mergeCell ref="E4:E29"/>
     <mergeCell ref="F4:F29"/>
-    <mergeCell ref="G4:G29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
recursos y seguimiento grado 05
</commit_message>
<xml_diff>
--- a/seguimiento/ProduccionDigital/SegDigital_MA_05_01_CO.xlsx
+++ b/seguimiento/ProduccionDigital/SegDigital_MA_05_01_CO.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="71">
   <si>
     <t>Cuaderno de estudio</t>
   </si>
@@ -765,7 +765,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -777,7 +777,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J4" sqref="J4"/>
+      <selection pane="topRight" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1174,7 +1174,9 @@
       <c r="H15" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="I15" s="17"/>
+      <c r="I15" s="17" t="s">
+        <v>67</v>
+      </c>
       <c r="J15" s="17"/>
       <c r="K15" s="22"/>
       <c r="L15" s="23"/>
@@ -1200,8 +1202,12 @@
       <c r="H16" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
+      <c r="I16" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="J16" s="16" t="s">
+        <v>67</v>
+      </c>
       <c r="K16" s="22"/>
       <c r="L16" s="23"/>
     </row>

</xml_diff>

<commit_message>
recursos 05 - actualización archivo seguimiento
</commit_message>
<xml_diff>
--- a/seguimiento/ProduccionDigital/SegDigital_MA_05_01_CO.xlsx
+++ b/seguimiento/ProduccionDigital/SegDigital_MA_05_01_CO.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="71">
   <si>
     <t>Cuaderno de estudio</t>
   </si>
@@ -777,7 +777,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J15" sqref="J15"/>
+      <selection pane="topRight" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -925,7 +925,9 @@
       <c r="I6" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="J6" s="16"/>
+      <c r="J6" s="16" t="s">
+        <v>67</v>
+      </c>
       <c r="K6" s="22"/>
       <c r="L6" s="23"/>
     </row>
@@ -953,7 +955,9 @@
       <c r="I7" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="17"/>
+      <c r="J7" s="17" t="s">
+        <v>67</v>
+      </c>
       <c r="K7" s="22"/>
       <c r="L7" s="23"/>
     </row>
@@ -981,7 +985,9 @@
       <c r="I8" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="J8" s="16"/>
+      <c r="J8" s="16" t="s">
+        <v>67</v>
+      </c>
       <c r="K8" s="22"/>
       <c r="L8" s="23"/>
     </row>
@@ -1037,7 +1043,9 @@
       <c r="I10" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="J10" s="16"/>
+      <c r="J10" s="16" t="s">
+        <v>67</v>
+      </c>
       <c r="K10" s="22"/>
       <c r="L10" s="23"/>
     </row>
@@ -1065,7 +1073,9 @@
       <c r="I11" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="J11" s="17"/>
+      <c r="J11" s="17" t="s">
+        <v>67</v>
+      </c>
       <c r="K11" s="22"/>
       <c r="L11" s="23"/>
     </row>
@@ -1093,7 +1103,9 @@
       <c r="I12" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="J12" s="16"/>
+      <c r="J12" s="16" t="s">
+        <v>67</v>
+      </c>
       <c r="K12" s="22"/>
       <c r="L12" s="23"/>
     </row>
@@ -1121,7 +1133,9 @@
       <c r="I13" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="J13" s="17"/>
+      <c r="J13" s="17" t="s">
+        <v>67</v>
+      </c>
       <c r="K13" s="22"/>
       <c r="L13" s="23"/>
     </row>
@@ -1177,7 +1191,9 @@
       <c r="I15" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="J15" s="17"/>
+      <c r="J15" s="17" t="s">
+        <v>67</v>
+      </c>
       <c r="K15" s="22"/>
       <c r="L15" s="23"/>
     </row>
@@ -1232,8 +1248,12 @@
       <c r="H17" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
+      <c r="I17" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="J17" s="17" t="s">
+        <v>67</v>
+      </c>
       <c r="K17" s="22"/>
       <c r="L17" s="23"/>
     </row>
@@ -1258,8 +1278,12 @@
       <c r="H18" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
+      <c r="I18" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="J18" s="16" t="s">
+        <v>67</v>
+      </c>
       <c r="K18" s="22"/>
       <c r="L18" s="23"/>
     </row>

</xml_diff>

<commit_message>
Actualización seguimiento grado 05
</commit_message>
<xml_diff>
--- a/seguimiento/ProduccionDigital/SegDigital_MA_05_01_CO.xlsx
+++ b/seguimiento/ProduccionDigital/SegDigital_MA_05_01_CO.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="71">
   <si>
     <t>Cuaderno de estudio</t>
   </si>
@@ -777,7 +777,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J18" sqref="J18"/>
+      <selection pane="topRight" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1308,8 +1308,12 @@
       <c r="H19" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
+      <c r="I19" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="J19" s="17" t="s">
+        <v>70</v>
+      </c>
       <c r="K19" s="22"/>
       <c r="L19" s="23"/>
     </row>
@@ -1334,8 +1338,12 @@
       <c r="H20" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
+      <c r="I20" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="J20" s="16" t="s">
+        <v>70</v>
+      </c>
       <c r="K20" s="22"/>
       <c r="L20" s="23"/>
     </row>
@@ -1360,7 +1368,9 @@
       <c r="H21" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="I21" s="17"/>
+      <c r="I21" s="17" t="s">
+        <v>68</v>
+      </c>
       <c r="J21" s="17"/>
       <c r="K21" s="22"/>
       <c r="L21" s="23"/>

</xml_diff>

<commit_message>
Actualización archivo seguimiento SegDigital_MA_05_01_CO
</commit_message>
<xml_diff>
--- a/seguimiento/ProduccionDigital/SegDigital_MA_05_01_CO.xlsx
+++ b/seguimiento/ProduccionDigital/SegDigital_MA_05_01_CO.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="72">
   <si>
     <t>Cuaderno de estudio</t>
   </si>
@@ -238,9 +238,6 @@
   </si>
   <si>
     <t>error</t>
-  </si>
-  <si>
-    <t>M102A no existe</t>
   </si>
 </sst>
 </file>
@@ -781,9 +778,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J29" sqref="J29"/>
+      <selection pane="topRight" activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1491,9 +1488,11 @@
         <v>67</v>
       </c>
       <c r="I25" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="J25" s="17"/>
+        <v>67</v>
+      </c>
+      <c r="J25" s="17" t="s">
+        <v>67</v>
+      </c>
       <c r="K25" s="22"/>
       <c r="L25" s="23"/>
     </row>

</xml_diff>